<commit_message>
finalize first test case
</commit_message>
<xml_diff>
--- a/src/test/java/testdata/data.xlsx
+++ b/src/test/java/testdata/data.xlsx
@@ -5,15 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\eclipse-workspace\HR-Framework\src\test\java\com\actitime\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\eclipse-workspace\test-automation-assignment-19550901\src\test\java\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2848C12D-97BE-4C06-977A-43DCE1B5EC5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EE3D341-B8A3-4BB6-99E6-62C313B55A40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-24195" yWindow="1365" windowWidth="18330" windowHeight="12480" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
+    <sheet name="Urls" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,12 +26,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>admin</t>
   </si>
   <si>
     <t>manager</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>https://demo.actitime.com/login.do</t>
+  </si>
+  <si>
+    <t>Dashboard</t>
+  </si>
+  <si>
+    <t>https://demo.actitime.com/user/submit_tt.do</t>
   </si>
 </sst>
 </file>
@@ -350,7 +363,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
@@ -367,4 +380,35 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4425896-7757-4284-A841-0175DD857F92}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add second third test cases
</commit_message>
<xml_diff>
--- a/src/test/java/testdata/data.xlsx
+++ b/src/test/java/testdata/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\eclipse-workspace\test-automation-assignment-19550901\src\test\java\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EE3D341-B8A3-4BB6-99E6-62C313B55A40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24D20E9E-63CB-4B21-BE1F-589D9ACE7ABC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-24195" yWindow="1365" windowWidth="18330" windowHeight="12480" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>admin</t>
   </si>
@@ -44,6 +44,18 @@
   </si>
   <si>
     <t>https://demo.actitime.com/user/submit_tt.do</t>
+  </si>
+  <si>
+    <t>Employee List Page</t>
+  </si>
+  <si>
+    <t>https://demo.actitime.com/administration/userlist.do</t>
+  </si>
+  <si>
+    <t>Time Track</t>
+  </si>
+  <si>
+    <t>https://demo.actitime.com/user/view_tt.do</t>
   </si>
 </sst>
 </file>
@@ -384,13 +396,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4425896-7757-4284-A841-0175DD857F92}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="29.21875" customWidth="1"/>
+    <col min="2" max="2" width="54.77734375" customWidth="1"/>
+    <col min="5" max="5" width="25.5546875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -406,6 +423,22 @@
       </c>
       <c r="B2" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added tes case four
</commit_message>
<xml_diff>
--- a/src/test/java/testdata/data.xlsx
+++ b/src/test/java/testdata/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\eclipse-workspace\test-automation-assignment-19550901\src\test\java\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24D20E9E-63CB-4B21-BE1F-589D9ACE7ABC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0915DA4B-75FC-4383-92CE-9635E4B8E50E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-24195" yWindow="1365" windowWidth="18330" windowHeight="12480" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>admin</t>
   </si>
@@ -56,6 +56,12 @@
   </si>
   <si>
     <t>https://demo.actitime.com/user/view_tt.do</t>
+  </si>
+  <si>
+    <t>https://demo.actitime.com/reports/reports.do</t>
+  </si>
+  <si>
+    <t>Reports</t>
   </si>
 </sst>
 </file>
@@ -396,10 +402,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4425896-7757-4284-A841-0175DD857F92}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -441,6 +447,14 @@
         <v>9</v>
       </c>
     </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>